<commit_message>
added more unit tests for read_excel and load_example_data to compensate for skipped doctests
because the later kind cannot be skipped when the required optional dependency is missing
</commit_message>
<xml_diff>
--- a/larray/tests/data/test.xlsx
+++ b/larray/tests/data/test.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Projects\larray\larray\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdm\devel\larray\larray\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{859F0767-2DB4-4DF8-8565-91DC024C7259}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5AFFA1-9C58-43F7-8F68-69C54A22109E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3015" windowWidth="21600" windowHeight="12735" activeTab="7" xr2:uid="{09308462-044D-43A2-BFAA-FA16022E58DA}"/>
+    <workbookView xWindow="4215" yWindow="2130" windowWidth="21600" windowHeight="11505" activeTab="4" xr2:uid="{09308462-044D-43A2-BFAA-FA16022E58DA}"/>
   </bookViews>
   <sheets>
     <sheet name="1d" sheetId="1" r:id="rId1"/>
     <sheet name="2d" sheetId="2" r:id="rId2"/>
     <sheet name="2d_classic" sheetId="3" r:id="rId3"/>
     <sheet name="3d" sheetId="4" r:id="rId4"/>
-    <sheet name="int_labels" sheetId="5" r:id="rId5"/>
-    <sheet name="missing_values" sheetId="6" r:id="rId6"/>
-    <sheet name="unsorted" sheetId="7" r:id="rId7"/>
-    <sheet name="position" sheetId="8" r:id="rId8"/>
+    <sheet name="3d_classic" sheetId="9" r:id="rId5"/>
+    <sheet name="int_labels" sheetId="5" r:id="rId6"/>
+    <sheet name="missing_values" sheetId="6" r:id="rId7"/>
+    <sheet name="unsorted" sheetId="7" r:id="rId8"/>
+    <sheet name="position" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="13">
   <si>
     <t>a</t>
   </si>
@@ -74,6 +75,9 @@
   </si>
   <si>
     <t>c2</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -720,6 +724,138 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A9360C-3F56-426E-9231-E081137E8DA0}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAECE338-0430-4B70-99DE-76F3AEBD8295}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -902,7 +1038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C5398B-1EE4-49A9-99E4-B0EB57D279D8}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1000,7 +1136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E6C7CF-BBE3-4611-A470-441B3A104D5F}">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1132,11 +1268,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57AAE1E-0A99-4EB4-BF25-728B735FC1DE}">
   <dimension ref="D3:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>